<commit_message>
[File] api - 파일 조회 추가
</commit_message>
<xml_diff>
--- a/docs/mvc-starter 도메인 정의.xlsx
+++ b/docs/mvc-starter 도메인 정의.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ju-jinyoo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/J.Reo/Documents/dev/workspace-git-spring/mvc-starter/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B9BCF5-5275-C340-9F47-B2DA3726CDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C748A3-7F76-B747-8547-460FD51E48AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="27000" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
+    <workbookView xWindow="33600" yWindow="500" windowWidth="33600" windowHeight="26440" activeTab="1" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
   </bookViews>
   <sheets>
     <sheet name="도메인" sheetId="1" r:id="rId1"/>
-    <sheet name="보드" sheetId="3" r:id="rId2"/>
-    <sheet name="파일" sheetId="4" r:id="rId3"/>
-    <sheet name="회원" sheetId="8" r:id="rId4"/>
+    <sheet name="파일" sheetId="4" r:id="rId2"/>
+    <sheet name="회원" sheetId="8" r:id="rId3"/>
+    <sheet name="보드" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
   <si>
     <t>보드</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -63,22 +63,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>키를 통한 파일 다운로드</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GET /files/{fileKey}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Base64 Image 다운로드</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GET /images/{fileKey}/base64</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>회원 조회 - 단건</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -223,22 +207,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/users/{userKey}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>회원 생성</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/users</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원 수정</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>회원 삭제</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -247,23 +219,59 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/users/{userKey}/boards/attractive</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>내가 쓴 게시글 조회 - 목록</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/users/{userKey}/boards/mine</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>게시판(board)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>게시판</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 갱신</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 갱신 - 프로필</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/members/{memberId}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/members</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/members/{memberId}/profile</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/members/{memberId}/boards/attractive</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/members/{memberId}/boards/mine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 조회 - Base64 Image</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 조회 - 다운로드</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/files/{fileKey}/download</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/files/{fileKey}/base64</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -382,6 +390,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -393,9 +404,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD70B4A5-D1C1-2044-886A-0AE496EA7834}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -728,59 +736,59 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>56</v>
+      <c r="B2" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="7" t="s">
-        <v>55</v>
+      <c r="A4" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -800,6 +808,222 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E653F8-7AFE-694F-A8DB-5CDEC2558A92}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3"/>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00806A96-FA12-9E42-8A8C-A0B75B8FF27F}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3"/>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D4686F-A243-C64F-B901-E33899BC9916}">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -816,35 +1040,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3"/>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -852,13 +1076,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -866,13 +1090,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -880,13 +1104,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -894,13 +1118,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -908,13 +1132,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -922,13 +1146,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -936,13 +1160,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -950,13 +1174,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -964,13 +1188,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -978,13 +1202,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -992,13 +1216,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1006,13 +1230,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1020,13 +1244,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1034,215 +1258,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C2:D2"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E653F8-7AFE-694F-A8DB-5CDEC2558A92}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
-  <cols>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3"/>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="10"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C2:D2"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00806A96-FA12-9E42-8A8C-A0B75B8FF27F}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
-  <cols>
-    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3"/>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="10"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[File] delete file 테스트 구현
</commit_message>
<xml_diff>
--- a/docs/mvc-starter 도메인 정의.xlsx
+++ b/docs/mvc-starter 도메인 정의.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/J.Reo/Documents/dev/workspace-git-spring/mvc-starter/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC1A98A-CA45-784F-9D3E-879D29335363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBB08C2-3DCF-4742-93CC-0772ACCB419D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19400" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
+    <workbookView xWindow="33600" yWindow="500" windowWidth="33600" windowHeight="26420" activeTab="1" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
   </bookViews>
   <sheets>
     <sheet name="도메인" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
   <si>
     <t>보드</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -280,6 +280,58 @@
   </si>
   <si>
     <t>/api/v1.0/boards/{boardKey}/attractive</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 업로드 - base64</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 조회 - 단건</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 제거</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>서비스</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>INPUT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUTPUT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>외부 API</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일명, 컨텐트 타입, base64 문자열</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>File DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>File Entity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>없음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -321,7 +373,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -390,22 +442,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -421,6 +490,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -430,22 +505,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -764,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD70B4A5-D1C1-2044-886A-0AE496EA7834}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -783,88 +852,88 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="2"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -879,83 +948,151 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E653F8-7AFE-694F-A8DB-5CDEC2558A92}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3"/>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2"/>
+      <c r="B7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="3" t="s">
+      <c r="D7" s="10"/>
+      <c r="E7" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3">
+      <c r="F7" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E8" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="3">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E9" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="F9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -978,131 +1115,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="3"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1131,252 +1268,252 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5 16383:16383">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="11"/>
-      <c r="XFC1" s="15"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13"/>
+      <c r="XFC1" s="8"/>
     </row>
     <row r="2" spans="1:5 16383:16383">
-      <c r="A2" s="3"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5 16383:16383">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5 16383:16383">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5 16383:16383">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5 16383:16383">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5 16383:16383">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5 16383:16383">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5 16383:16383">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5 16383:16383">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5 16383:16383">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5 16383:16383">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5 16383:16383">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5 16383:16383">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5 16383:16383">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5 16383:16383">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
[Member / File] 외부 API 구현 및 테스트
</commit_message>
<xml_diff>
--- a/docs/mvc-starter 도메인 정의.xlsx
+++ b/docs/mvc-starter 도메인 정의.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/J.Reo/Documents/dev/workspace-git-spring/mvc-starter/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAEEB5F-5AD2-A64B-AE47-DABB6D44BC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE513811-255A-6542-97DC-603AC27FF953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="500" windowWidth="33600" windowHeight="26420" activeTab="2" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="97">
   <si>
     <t>보드</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -420,6 +420,10 @@
   </si>
   <si>
     <t>Comment DTO, Comment DTO Page</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>select 쿼리</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1023,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E653F8-7AFE-694F-A8DB-5CDEC2558A92}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:F7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1036,7 +1040,7 @@
     <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -1046,7 +1050,7 @@
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>51</v>
@@ -1064,7 +1068,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1082,7 +1086,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1100,7 +1104,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1118,7 +1122,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
         <v>54</v>
@@ -1133,8 +1137,11 @@
       <c r="F7" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1150,9 +1157,14 @@
       <c r="E8" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="F8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -1168,7 +1180,12 @@
       <c r="E9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1182,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00806A96-FA12-9E42-8A8C-A0B75B8FF27F}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1195,7 +1212,7 @@
     <col min="4" max="4" width="51.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
@@ -1205,7 +1222,7 @@
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>51</v>
@@ -1223,7 +1240,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1243,7 +1260,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1263,7 +1280,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1283,7 +1300,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1303,7 +1320,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1323,7 +1340,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" s="1"/>
       <c r="B9" s="3" t="s">
         <v>54</v>
@@ -1338,8 +1355,11 @@
       <c r="F9" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1352,10 +1372,17 @@
       <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="E10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -1368,10 +1395,17 @@
       <c r="D11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -1384,10 +1418,17 @@
       <c r="D12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="E12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -1400,10 +1441,17 @@
       <c r="D13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="E13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -1416,10 +1464,17 @@
       <c r="D14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="E14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>6</v>
       </c>
@@ -1434,8 +1489,9 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>7</v>
       </c>
@@ -1450,8 +1506,9 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>8</v>
       </c>
@@ -1466,6 +1523,7 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
[Member] ReqBody -> Dto 세분화 로 변경
</commit_message>
<xml_diff>
--- a/docs/mvc-starter 도메인 정의.xlsx
+++ b/docs/mvc-starter 도메인 정의.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/J.Reo/Documents/dev/workspace-git-spring/mvc-starter/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ju-jinyoo/Documents/dev/workspace-git-jujin/mvc-starter/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE513811-255A-6542-97DC-603AC27FF953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD3CB4E-1BA4-2A40-A934-944EE2AD5FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="500" windowWidth="33600" windowHeight="26420" activeTab="2" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
+    <workbookView xWindow="17600" yWindow="500" windowWidth="33600" windowHeight="26420" activeTab="1" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
   </bookViews>
   <sheets>
     <sheet name="도메인" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="99">
   <si>
     <t>보드</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -267,10 +267,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>File DTO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>File Entity</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -283,18 +279,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Member DTO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Member ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Member ID, Member DTO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>관심 게시글 조회 - 페이지</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -424,6 +412,26 @@
   </si>
   <si>
     <t>select 쿼리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member Create DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member ID, Member Update DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member ID, Member Update profile DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member Read DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>File Read DTO</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -982,7 +990,7 @@
     <row r="5" spans="1:2">
       <c r="A5" s="11"/>
       <c r="B5" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1029,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E653F8-7AFE-694F-A8DB-5CDEC2558A92}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1065,7 +1073,7 @@
         <v>45</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1079,7 +1087,7 @@
         <v>55</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
@@ -1097,7 +1105,7 @@
         <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
@@ -1115,7 +1123,7 @@
         <v>56</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
@@ -1135,10 +1143,10 @@
         <v>45</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1201,14 +1209,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00806A96-FA12-9E42-8A8C-A0B75B8FF27F}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1237,7 +1245,7 @@
         <v>45</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1248,10 +1256,10 @@
         <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>46</v>
@@ -1268,10 +1276,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>46</v>
@@ -1288,10 +1296,10 @@
         <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>46</v>
@@ -1308,10 +1316,10 @@
         <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>46</v>
@@ -1328,10 +1336,10 @@
         <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>46</v>
@@ -1353,10 +1361,10 @@
         <v>45</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1479,7 +1487,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>26</v>
@@ -1496,7 +1504,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>26</v>
@@ -1513,13 +1521,13 @@
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1576,7 +1584,7 @@
         <v>45</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6 16383:16383">
@@ -1587,10 +1595,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1600,13 +1608,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1619,10 +1627,10 @@
         <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1632,13 +1640,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1651,10 +1659,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1667,10 +1675,10 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1683,10 +1691,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1696,13 +1704,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1715,10 +1723,10 @@
         <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1731,10 +1739,10 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1747,10 +1755,10 @@
         <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1763,10 +1771,10 @@
         <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1779,10 +1787,10 @@
         <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1795,10 +1803,10 @@
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1811,10 +1819,10 @@
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1824,13 +1832,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1840,13 +1848,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1864,7 +1872,7 @@
         <v>45</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1910,7 +1918,7 @@
         <v>26</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1920,13 +1928,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1942,7 +1950,7 @@
         <v>29</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1958,7 +1966,7 @@
         <v>27</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1974,7 +1982,7 @@
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1990,7 +1998,7 @@
         <v>26</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2006,7 +2014,7 @@
         <v>26</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -2022,7 +2030,7 @@
         <v>27</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -2038,7 +2046,7 @@
         <v>28</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2054,7 +2062,7 @@
         <v>29</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2070,7 +2078,7 @@
         <v>27</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2086,7 +2094,7 @@
         <v>27</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>

</xml_diff>

<commit_message>
[File] FileService 구현 및 테스트 완료
</commit_message>
<xml_diff>
--- a/docs/mvc-starter 도메인 정의.xlsx
+++ b/docs/mvc-starter 도메인 정의.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ju-jinyoo/Documents/dev/workspace-git-jujin/mvc-starter/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ED51FC-F898-AD43-9E51-37448E97B37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA18601-3B4B-AB43-A12C-8F6B0D4F23BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53340" yWindow="-240" windowWidth="33600" windowHeight="21100" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
+    <workbookView xWindow="53340" yWindow="-240" windowWidth="33600" windowHeight="21100" activeTab="1" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
   </bookViews>
   <sheets>
     <sheet name="도메인" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="108">
   <si>
     <t>보드</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -983,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD70B4A5-D1C1-2044-886A-0AE496EA7834}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1087,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E653F8-7AFE-694F-A8DB-5CDEC2558A92}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1157,8 +1157,12 @@
       <c r="D4" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
@@ -1173,8 +1177,12 @@
       <c r="D5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">

</xml_diff>

<commit_message>
[Board] Board Service 설계
</commit_message>
<xml_diff>
--- a/docs/mvc-starter 도메인 정의.xlsx
+++ b/docs/mvc-starter 도메인 정의.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ju-jinyoo/Documents/dev/workspace-git-jujin/mvc-starter/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA18601-3B4B-AB43-A12C-8F6B0D4F23BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046375EB-D62E-9349-B24E-F77E917E7E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53340" yWindow="-240" windowWidth="33600" windowHeight="21100" activeTab="1" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
+    <workbookView xWindow="53340" yWindow="-240" windowWidth="33600" windowHeight="21100" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
   </bookViews>
   <sheets>
     <sheet name="도메인" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="117">
   <si>
     <t>보드</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -431,10 +431,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Comment Read DTO, Comment Read DTO Page</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Board ID, Comment ID, Comment Create DTO</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -468,6 +464,46 @@
   </si>
   <si>
     <t>나의 댓글(my comments)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 업로드 - Multipart - 여러건</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일 업로드 - Multipart - 단건</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>File Entity List</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MultipartFile List</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MultipartFile</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Board Topic, Pageble</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Board ID, ReportReason</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>신고(report)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원(member)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardReport</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -981,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD70B4A5-D1C1-2044-886A-0AE496EA7834}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1026,7 +1062,7 @@
     <row r="4" spans="1:3">
       <c r="A4" s="11"/>
       <c r="B4" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1053,30 +1089,39 @@
     <row r="7" spans="1:3">
       <c r="A7" s="11"/>
       <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>114</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="11"/>
       <c r="B8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A6:A9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1085,15 +1130,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E653F8-7AFE-694F-A8DB-5CDEC2558A92}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1147,131 +1192,165 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1"/>
-      <c r="B8" s="3" t="s">
+      <c r="E8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="3" t="s">
+      <c r="D10" s="12"/>
+      <c r="E10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G10" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1">
+    <row r="11" spans="1:7">
+      <c r="A11" s="1">
         <v>1</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="E11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1">
+    <row r="12" spans="1:7">
+      <c r="A12" s="1">
         <v>2</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="E12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1619,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D4686F-A243-C64F-B901-E33899BC9916}">
-  <dimension ref="A1:XFC36"/>
+  <dimension ref="A1:XFC35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1701,7 +1780,7 @@
         <v>93</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>95</v>
@@ -1714,13 +1793,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1781,7 +1860,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>52</v>
@@ -1807,26 +1886,26 @@
     </row>
     <row r="12" spans="1:6 16383:16383">
       <c r="A12" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6 16383:16383">
       <c r="A13" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>99</v>
@@ -1839,13 +1918,13 @@
     </row>
     <row r="14" spans="1:6 16383:16383">
       <c r="A14" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>52</v>
@@ -1855,13 +1934,13 @@
     </row>
     <row r="15" spans="1:6 16383:16383">
       <c r="A15" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>52</v>
@@ -1871,13 +1950,13 @@
     </row>
     <row r="16" spans="1:6 16383:16383">
       <c r="A16" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>52</v>
@@ -1887,13 +1966,13 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>52</v>
@@ -1903,26 +1982,26 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>57</v>
@@ -1933,79 +2012,79 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="1">
-        <v>17</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1"/>
+      <c r="B21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="1"/>
-      <c r="B22" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
-        <v>2</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
-        <v>3</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>23</v>
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>65</v>
@@ -2015,13 +2094,13 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>65</v>
@@ -2031,109 +2110,109 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>69</v>
@@ -2143,56 +2222,40 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="1">
-        <v>14</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Domain - Board] Board 도메인 관련 서비스 및 API 조립 완료
</commit_message>
<xml_diff>
--- a/docs/mvc-starter 도메인 정의.xlsx
+++ b/docs/mvc-starter 도메인 정의.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/J.Reo/Documents/dev/workspace-git-spring/mvc-starter/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ju-jinyoo/Documents/dev/workspace-git-jujin/mvc-starter/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384F8C4A-A098-784E-A30F-010C67A5A781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490970F8-DADA-2444-9C04-0E803CE8E9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="26420" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
+    <workbookView xWindow="51200" yWindow="-240" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
   </bookViews>
   <sheets>
     <sheet name="도메인" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="109">
   <si>
     <t>파일</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -67,18 +67,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>게시글 댓글 저장</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>게시글 댓글 수정</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>게시글 숨김 처리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>게시글 댓글 삭제</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -91,14 +83,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>게시글 댓글 및 대댓글 조회</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시글 댓글 숨김 처리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>GET</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -275,10 +259,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>게시글 상세 조회 - 단건</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>파일 리소스 조회 - 단건</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -311,14 +291,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Post Create DTO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Post ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>게시글 신규</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -331,34 +303,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Post ID, Post Update DTO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Post ID, IsHide</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Post ID, Pageble</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Post ID, Comment ID, Comment Create DTO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Post ID, Comment ID, Comment Update DTO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Post ID, Comment ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Post ID, Comment ID, IsHide</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/v1.0/boards/{boardId}/posts</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -367,10 +315,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/api/v1.0/boards/{boardId}/posts/{postId}/hide</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>/api/v1.0/boards/{boardId}/posts/{postId}/comments</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -427,18 +371,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>관심 게시판 조회</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>관심 게시글 조회</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>내가 쓴 게시글 조회</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Member ID, Post ID, isLiked</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -451,10 +383,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>내가 쓴 게시글의 댓글 조회</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Member ID, Page</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -488,6 +416,62 @@
   </si>
   <si>
     <t>회원 댓글(memberComment)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>내가 쓴 게시글의 댓글 조회 - 페이지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Board ID, Post ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Board ID, Pageble</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member ID, Post ID, Post Update DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member ID, Post ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 댓글 신규</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member ID, Comment ID, Comment Update DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member ID, Comment ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 신규</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member ID, Post ID, Parent Comment ID, Comment Create DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member ID, Board ID, Post Create DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 대댓글 신규</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 댓글 및 대댓글 조회 - 페이지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Member ID, Post ID, Comment Create DTO</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -665,7 +649,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -699,6 +683,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -717,6 +707,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -724,9 +717,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1045,7 +1035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD70B4A5-D1C1-2044-886A-0AE496EA7834}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1060,47 +1050,47 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="11"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="5" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="11"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="5" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="12" t="s">
-        <v>21</v>
+      <c r="A5" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="13"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="13"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1108,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1137,31 +1127,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1169,19 +1159,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1189,19 +1179,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1209,19 +1199,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1229,19 +1219,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1249,38 +1239,38 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1"/>
       <c r="B9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="14"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1288,19 +1278,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G10" s="1">
         <v>1</v>
@@ -1311,19 +1301,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>
@@ -1344,7 +1334,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:D23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1355,31 +1345,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="A1" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1387,19 +1377,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1410,16 +1400,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1427,19 +1417,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1447,19 +1437,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1467,47 +1457,47 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
+      <c r="A8" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1515,13 +1505,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1531,13 +1521,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1547,13 +1537,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1563,13 +1553,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1579,13 +1569,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1593,20 +1583,20 @@
     <row r="16" spans="1:7">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="14"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1614,19 +1604,19 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G17" s="1">
         <v>0</v>
@@ -1640,16 +1630,16 @@
         <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G18" s="1">
         <v>1</v>
@@ -1660,19 +1650,19 @@
         <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G19" s="1">
         <v>1</v>
@@ -1683,19 +1673,19 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G20" s="1">
         <v>1</v>
@@ -1706,19 +1696,19 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G21" s="1">
         <v>1</v>
@@ -1729,13 +1719,13 @@
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1746,13 +1736,13 @@
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1763,13 +1753,13 @@
         <v>8</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1780,13 +1770,13 @@
         <v>9</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1797,13 +1787,13 @@
         <v>10</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1822,47 +1812,47 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D4686F-A243-C64F-B901-E33899BC9916}">
-  <dimension ref="A1:XFC30"/>
+  <dimension ref="A1:XFC29"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6 16383:16383">
-      <c r="A1" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="A1" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
       <c r="XFC1" s="7"/>
     </row>
     <row r="2" spans="1:6 16383:16383">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6 16383:16383">
@@ -1870,39 +1860,39 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6 16383:16383">
-      <c r="A4" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="19"/>
+      <c r="A4" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="1:6 16383:16383">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1912,13 +1902,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1928,13 +1918,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1944,13 +1934,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1963,336 +1953,321 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6 16383:16383">
-      <c r="A10" s="1">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="A10" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
     </row>
     <row r="11" spans="1:6 16383:16383">
-      <c r="A11" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19"/>
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6 16383:16383">
       <c r="A12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6 16383:16383">
       <c r="A13" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6 16383:16383">
       <c r="A14" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6 16383:16383">
       <c r="A15" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6 16383:16383">
-      <c r="A16" s="1">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1"/>
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="1"/>
-      <c r="B18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>3</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>4</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="1">
-        <v>11</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A10:F10"/>
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[설계] Controller 에 API 타입 및 INPUT/OUTPUT 추가
</commit_message>
<xml_diff>
--- a/docs/mvc-starter 도메인 정의.xlsx
+++ b/docs/mvc-starter 도메인 정의.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ju-jinyoo/Documents/dev/workspace-git-jujin/mvc-starter/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95684E12-AF76-594F-8CEB-BB86A5BBD501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C42FE1-9A97-7C48-84CF-DC633DB096C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51220" yWindow="-240" windowWidth="38400" windowHeight="21100" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
+    <workbookView xWindow="51200" yWindow="-240" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
   </bookViews>
   <sheets>
     <sheet name="도메인" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="124">
   <si>
     <t>파일</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -51,10 +51,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>url</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>회원 조회 - 단건</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -504,6 +500,38 @@
   </si>
   <si>
     <t>회원 게시판(memberBoard)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>METHOD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BoardApiController</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MemberApiController</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FileApiController</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Restful</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Functional</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>API Type(Restful / Functional)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -701,6 +729,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -719,14 +750,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1044,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD70B4A5-D1C1-2044-886A-0AE496EA7834}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1059,41 +1087,41 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="13"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="14" t="s">
-        <v>17</v>
+      <c r="A4" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="16"/>
+      <c r="B5" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="16"/>
+      <c r="B6" s="1" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="15"/>
-      <c r="B6" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1101,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1116,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E653F8-7AFE-694F-A8DB-5CDEC2558A92}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1127,15 +1155,16 @@
     <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="17"/>
       <c r="C1" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1143,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1152,7 +1181,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1161,7 +1190,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1170,7 +1199,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -1179,7 +1208,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1188,37 +1217,37 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:6" s="21" customFormat="1"/>
+    <row r="8" spans="1:6" s="13" customFormat="1"/>
     <row r="9" spans="1:6">
-      <c r="A9" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="A9" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1226,19 +1255,19 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1246,19 +1275,19 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1266,19 +1295,19 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1286,19 +1315,19 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1306,91 +1335,123 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1"/>
+      <c r="B18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="1"/>
-      <c r="B17" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="1">
+      <c r="J18" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1">
         <v>1</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="F19" s="6"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="1">
-        <v>2</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="1">
+      <c r="F20" s="6"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C17:D17"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A17:G17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1399,26 +1460,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00806A96-FA12-9E42-8A8C-A0B75B8FF27F}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="18" t="s">
-        <v>107</v>
+      <c r="A1" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1426,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1435,7 +1497,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1444,7 +1506,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1453,7 +1515,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -1462,7 +1524,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1471,41 +1533,41 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="A9" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1513,19 +1575,19 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1533,19 +1595,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1553,19 +1615,19 @@
         <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1573,19 +1635,19 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1593,354 +1655,426 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="A16" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="E17" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="6">
         <v>1</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:10">
       <c r="A19" s="6">
         <v>2</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:10">
       <c r="A20" s="6">
         <v>3</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:10">
       <c r="A21" s="6">
         <v>4</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:10">
       <c r="A22" s="6">
         <v>5</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="1"/>
-      <c r="B24" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" s="16" t="s">
+    <row r="24" spans="1:10">
+      <c r="A24" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1"/>
+      <c r="B25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="1">
+      <c r="C27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27" s="1">
         <v>1</v>
       </c>
-      <c r="B25" s="1" t="s">
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1">
+        <v>3</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="1">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="1">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="1">
-        <v>2</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="1">
-        <v>3</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="1">
-        <v>4</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="1">
-        <v>5</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="1">
-        <v>6</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E31" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
-        <v>10</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>73</v>
+        <v>9</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="1">
+        <v>10</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C24:D24"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A16:F16"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A24:G24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1949,27 +2083,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D4686F-A243-C64F-B901-E33899BC9916}">
-  <dimension ref="A1:XFC37"/>
+  <dimension ref="A1:XFC38"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6 16383:16383">
-      <c r="A1" s="18" t="s">
-        <v>107</v>
+      <c r="A1" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6 16383:16383">
@@ -1977,7 +2112,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1986,7 +2121,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1995,7 +2130,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -2004,7 +2139,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -2013,7 +2148,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -2022,37 +2157,37 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="9" spans="1:6 16383:16383">
-      <c r="A9" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="A9" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
       <c r="XFC9" s="7"/>
     </row>
     <row r="10" spans="1:6 16383:16383">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>34</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6 16383:16383">
@@ -2060,25 +2195,25 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6 16383:16383">
-      <c r="A12" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="A12" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6 16383:16383">
@@ -2086,13 +2221,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2102,13 +2237,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2118,13 +2253,13 @@
         <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -2134,335 +2269,416 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+    <row r="18" spans="1:9">
+      <c r="A18" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="20"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="1"/>
-      <c r="B25" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="1">
+    <row r="25" spans="1:9">
+      <c r="A25" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1"/>
+      <c r="B26" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1">
         <v>1</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="1">
-        <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="1">
+        <v>2</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="1">
+        <v>3</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="1">
+        <v>4</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="1">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="1">
-        <v>3</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="1">
+        <v>6</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="1">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="1">
-        <v>4</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="E33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="1">
+        <v>8</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="1">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="1">
+        <v>10</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="1">
+        <v>11</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="1">
-        <v>5</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="C37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="1">
+        <v>12</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="1">
-        <v>6</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="1">
-        <v>7</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="1">
-        <v>8</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="1">
-        <v>9</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="1">
-        <v>10</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="1">
-        <v>11</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="1">
-        <v>12</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A25:F25"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C25:D25"/>
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A9:F9"/>

</xml_diff>

<commit_message>
[User] Member -> User 변경
</commit_message>
<xml_diff>
--- a/docs/mvc-starter 도메인 정의.xlsx
+++ b/docs/mvc-starter 도메인 정의.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ju-jinyoo/Documents/dev/workspace-git-jujin/mvc-starter/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/J.Reo/Documents/dev/workspace-git-spring/mvc-starter/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C42FE1-9A97-7C48-84CF-DC633DB096C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902B4770-1D38-4445-873B-84B02FF8E19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="-240" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
+    <workbookView xWindow="-20" yWindow="520" windowWidth="48500" windowHeight="26440" activeTab="3" xr2:uid="{3D6FD482-1C04-F448-8517-59EBDEE51B15}"/>
   </bookViews>
   <sheets>
     <sheet name="도메인" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="148">
   <si>
     <t>파일</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -115,18 +115,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/api/v1.0/members/{memberId}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/v1.0/members</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/v1.0/members/{memberId}/profile</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>파일 조회 - 다운로드</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -195,10 +183,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Member ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>관심 게시글 조회 - 페이지</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -227,26 +211,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Member Create DTO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Member ID, Member Update DTO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Member ID, Member Update profile DTO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Member Read DTO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/v1.0/members/{memberId}/boards/like</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Board Read DTO Page</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -271,10 +235,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>회원(member)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>파일 업로드 - Multipart</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -331,38 +291,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/api/v1.0/members/{memberId}/boards/posts/comments/mine</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/v1.0/members/{memberId}/boards/posts/{postId}/like</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/v1.0/members/{memberId}/boards/posts/mine</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/v1.0/members/{memberId}/boards/posts/like</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>관심 게시판 조회 - 페이지</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>MemberService</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemberBoardService</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Member ID, Post ID, isLiked</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>BoardPost Read DTO Page</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -371,10 +303,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Member ID, Page</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>BoardService</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -451,10 +379,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>게시글 댓글 및 대댓글 조회 - 페이지</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Member ID, Post ID, Comment Create DTO</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -499,10 +423,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>회원 게시판(memberBoard)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>URL</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -515,10 +435,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>MemberApiController</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>FileApiController</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -532,6 +448,179 @@
   </si>
   <si>
     <t>API Type(Restful / Functional)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 조회 - 슬라이스</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/boards/{boardId}/posts/slice</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/boards/{boardId}/posts/paging</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원(user)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 게시판(userBoard)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserService</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserBoardService</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserApiController</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/users</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/users/{userId}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/users/{userId}/profile</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/users/{userId}/boards/like</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/users/{userId}/boards/posts/like</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/users/{userId}/boards/posts/mine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/users/{userId}/boards/posts/{postId}/like</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/users/{userId}/boards/posts/comments/mine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Post Create DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Post ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Post Read DTO Page</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Post Read DTO Slice</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Post Read DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Post Update DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment Create DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 댓글 조회 - 슬라이스</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/boards/{boardId}/posts/{postId}/comments/paging</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1.0/boards/{boardId}/posts/{postId}/comments/slice</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment Read DTO Page</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment Read DTO Slice</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment Update DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resource</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Create DTO</t>
+  </si>
+  <si>
+    <t>User Create DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>User Read DTO</t>
+  </si>
+  <si>
+    <t>User ID, User Update DTO</t>
+  </si>
+  <si>
+    <t>User ID, User Update profile DTO</t>
+  </si>
+  <si>
+    <t>User ID, Page</t>
+  </si>
+  <si>
+    <t>User ID, Post ID, isLiked</t>
+  </si>
+  <si>
+    <t>User ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Read DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>User Update DTO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>profile(base64 string)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>isLiked(boolean)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pageable</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -689,7 +778,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -755,6 +844,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1073,7 +1183,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1095,13 +1205,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="14"/>
       <c r="B3" s="5" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1109,19 +1219,19 @@
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="16"/>
       <c r="B5" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="16"/>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1146,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E653F8-7AFE-694F-A8DB-5CDEC2558A92}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1156,15 +1266,16 @@
     <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="17" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="3" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1172,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1181,7 +1292,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1190,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1199,7 +1310,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -1208,7 +1319,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1217,14 +1328,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:6" s="13" customFormat="1"/>
     <row r="9" spans="1:6">
       <c r="A9" s="17" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -1235,19 +1346,19 @@
     <row r="10" spans="1:6">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1255,19 +1366,19 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1275,19 +1386,19 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1295,19 +1406,19 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1315,19 +1426,19 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1335,24 +1446,24 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="17" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -1364,31 +1475,31 @@
     <row r="18" spans="1:10">
       <c r="A18" s="1"/>
       <c r="B18" s="3" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1396,24 +1507,28 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="H19" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J19" s="1">
         <v>1</v>
@@ -1424,24 +1539,28 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="H20" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J20" s="1">
         <v>1</v>
@@ -1460,10 +1579,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00806A96-FA12-9E42-8A8C-A0B75B8FF27F}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1472,15 +1591,17 @@
     <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="19" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="3" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1488,7 +1609,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1497,7 +1618,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1506,7 +1627,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1515,7 +1636,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -1524,7 +1645,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1533,7 +1654,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -1544,7 +1665,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="17" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -1555,19 +1676,19 @@
     <row r="10" spans="1:6">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1575,19 +1696,19 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>134</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1598,16 +1719,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>50</v>
+        <v>137</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1618,16 +1739,16 @@
         <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1638,16 +1759,16 @@
         <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>49</v>
+        <v>139</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1658,246 +1779,234 @@
         <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="A17" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="6">
-        <v>1</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>83</v>
+        <v>140</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>83</v>
+        <v>140</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
+    <row r="23" spans="1:10">
+      <c r="A23" s="6">
+        <v>5</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="1"/>
-      <c r="B25" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>46</v>
-      </c>
+      <c r="A25" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="1">
-        <v>1</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J26" s="1">
-        <v>0</v>
+      <c r="A26" s="1"/>
+      <c r="B26" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+        <v>111</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="H27" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1">
+        <v>2</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="H28" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J28" s="1">
         <v>1</v>
@@ -1905,27 +2014,31 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H29" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J29" s="1">
         <v>1</v>
@@ -1933,27 +2046,31 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
+        <v>113</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H30" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J30" s="1">
         <v>1</v>
@@ -1961,120 +2078,172 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+        <v>114</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1">
-        <v>10</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>72</v>
+        <v>9</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="1">
+        <v>10</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:F17"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A25:G25"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2083,9 +2252,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D4686F-A243-C64F-B901-E33899BC9916}">
-  <dimension ref="A1:XFC38"/>
+  <dimension ref="A1:XFC41"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -2096,15 +2265,17 @@
     <col min="3" max="3" width="51" customWidth="1"/>
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6 16383:16383">
       <c r="A1" s="19" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="3" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6 16383:16383">
@@ -2112,7 +2283,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -2121,7 +2292,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -2130,7 +2301,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -2139,7 +2310,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -2148,7 +2319,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -2157,13 +2328,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="9" spans="1:6 16383:16383">
       <c r="A9" s="17" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -2175,19 +2346,19 @@
     <row r="10" spans="1:6 16383:16383">
       <c r="A10" s="1"/>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6 16383:16383">
@@ -2195,492 +2366,581 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6 16383:16383">
-      <c r="A12" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="20"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="26"/>
     </row>
     <row r="13" spans="1:6 16383:16383">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="A13" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:6 16383:16383">
       <c r="A14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6 16383:16383">
       <c r="A15" s="1">
-        <v>3</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>89</v>
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6 16383:16383">
       <c r="A16" s="1">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>94</v>
+        <v>3</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="20"/>
+      <c r="A18" s="1">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="27"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="1">
-        <v>2</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
+      <c r="A20" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="20"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="1"/>
-      <c r="B26" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A25" s="1">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="1">
-        <v>1</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="A27" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="1">
-        <v>2</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1">
-        <v>4</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1">
-        <v>7</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>96</v>
+        <v>5</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>11</v>
+        <v>100</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E37" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="1">
+        <v>11</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="1">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="1">
+        <v>13</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A27:F27"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A20:F20"/>
     <mergeCell ref="A9:F9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>